<commit_message>
Kenya cleaned and comparing poverty
</commit_message>
<xml_diff>
--- a/Mozambique/input/Mozambique Spending_health per capita and education per student 2018.xlsx
+++ b/Mozambique/input/Mozambique Spending_health per capita and education per student 2018.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\git\subnational_need_resources\Mozambique\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{890A75E0-726E-422C-BB2B-60EEBB92F075}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBD2CDB9-42C0-4DC9-9A63-8D64B3AEDA21}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24720" windowHeight="12170" xr2:uid="{2C1E8659-3F79-4015-9906-A60AC24606A9}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4548" uniqueCount="882">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4550" uniqueCount="884">
   <si>
     <t>Province</t>
   </si>
@@ -5728,6 +5728,12 @@
   </si>
   <si>
     <t>Government own revenue spending on education (2018 budget US$/child)</t>
+  </si>
+  <si>
+    <t>Government own revenue spending on health (2018 budget US$)</t>
+  </si>
+  <si>
+    <t>Government own revenue spending on education (2018 budget US$)</t>
   </si>
 </sst>
 </file>
@@ -6442,10 +6448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD55168C-C206-40BF-9349-A828BA7B3CE3}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -6455,157 +6461,229 @@
     <col min="3" max="3" width="18.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="58">
+    <row r="1" spans="1:5" ht="58">
       <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="52" t="s">
+        <v>882</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>883</v>
+      </c>
+      <c r="D1" t="s">
         <v>881</v>
       </c>
-      <c r="C1" s="52" t="s">
+      <c r="E1" t="s">
         <v>881</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:5">
       <c r="A2" s="43" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="49">
-        <f>(('P. Totals'!J4+'P. Totals'!K4)/ER!$G$7/'Population data'!C19)*1000</f>
+        <f>(('P. Totals'!J4+'P. Totals'!K4)/ER!$G$7)*1000</f>
+        <v>13795620.668196464</v>
+      </c>
+      <c r="C2" s="49">
+        <f>(('P. Totals'!D4+'P. Totals'!E4)/ER!$G$7)*1000</f>
+        <v>38763237.566926554</v>
+      </c>
+      <c r="D2">
         <v>11.783243067414256</v>
       </c>
-      <c r="C2" s="49">
-        <f>(('P. Totals'!D4+'P. Totals'!E4)/ER!$G$7/Education!I10)*1000</f>
+      <c r="E2">
         <v>98.807923261833281</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:5">
       <c r="A3" s="43" t="s">
         <v>66</v>
       </c>
       <c r="B3" s="49">
-        <f>(('P. Totals'!J5+'P. Totals'!K5)/ER!$G$7/'Population data'!C20)*1000</f>
+        <f>(('P. Totals'!J5+'P. Totals'!K5)/ER!$G$7)*1000</f>
+        <v>17016862.794034287</v>
+      </c>
+      <c r="C3" s="49">
+        <f>(('P. Totals'!D5+'P. Totals'!E5)/ER!$G$7)*1000</f>
+        <v>41790352.176405646</v>
+      </c>
+      <c r="D3">
         <v>10.592058844713881</v>
       </c>
-      <c r="C3" s="49">
-        <f>(('P. Totals'!D5+'P. Totals'!E5)/ER!$G$7/Education!I11)*1000</f>
+      <c r="E3">
         <v>96.218637515986003</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:5">
       <c r="A4" s="43" t="s">
         <v>138</v>
       </c>
       <c r="B4" s="49">
-        <f>(('P. Totals'!J6+'P. Totals'!K6)/ER!$G$7/'Population data'!C21)*1000</f>
+        <f>(('P. Totals'!J6+'P. Totals'!K6)/ER!$G$7)*1000</f>
+        <v>30366522.987529583</v>
+      </c>
+      <c r="C4" s="49">
+        <f>(('P. Totals'!D6+'P. Totals'!E6)/ER!$G$7)*1000</f>
+        <v>94976064.128090248</v>
+      </c>
+      <c r="D4">
         <v>7.6190345092535532</v>
       </c>
-      <c r="C4" s="49">
-        <f>(('P. Totals'!D6+'P. Totals'!E6)/ER!$G$7/Education!I12)*1000</f>
+      <c r="E4">
         <v>77.814025234558002</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:5">
       <c r="A5" s="43" t="s">
         <v>183</v>
       </c>
       <c r="B5" s="49">
-        <f>(('P. Totals'!J7+'P. Totals'!K7)/ER!$G$7/'Population data'!C22)*1000</f>
+        <f>(('P. Totals'!J7+'P. Totals'!K7)/ER!$G$7)*1000</f>
+        <v>31812598.790747628</v>
+      </c>
+      <c r="C5" s="49">
+        <f>(('P. Totals'!D7+'P. Totals'!E7)/ER!$G$7)*1000</f>
+        <v>103210958.68513691</v>
+      </c>
+      <c r="D5">
         <v>8.264182537722256</v>
       </c>
-      <c r="C5" s="49">
-        <f>(('P. Totals'!D7+'P. Totals'!E7)/ER!$G$7/Education!I13)*1000</f>
+      <c r="E5">
         <v>64.143396656903377</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:5">
       <c r="A6" s="43" t="s">
         <v>233</v>
       </c>
       <c r="B6" s="49">
-        <f>(('P. Totals'!J8+'P. Totals'!K8)/ER!$G$7/'Population data'!C23)*1000</f>
+        <f>(('P. Totals'!J8+'P. Totals'!K8)/ER!$G$7)*1000</f>
+        <v>13569601.507239604</v>
+      </c>
+      <c r="C6" s="49">
+        <f>(('P. Totals'!D8+'P. Totals'!E8)/ER!$G$7)*1000</f>
+        <v>44480790.222011171</v>
+      </c>
+      <c r="D6">
         <v>7.6064195734784352</v>
       </c>
-      <c r="C6" s="49">
-        <f>(('P. Totals'!D8+'P. Totals'!E8)/ER!$G$7/Education!I14)*1000</f>
+      <c r="E6">
         <v>72.883722742023025</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:5">
       <c r="A7" s="43" t="s">
         <v>319</v>
       </c>
       <c r="B7" s="49">
-        <f>(('P. Totals'!J9+'P. Totals'!K9)/ER!$G$7/'Population data'!C24)*1000</f>
+        <f>(('P. Totals'!J9+'P. Totals'!K9)/ER!$G$7)*1000</f>
+        <v>14878688.566946441</v>
+      </c>
+      <c r="C7" s="49">
+        <f>(('P. Totals'!D9+'P. Totals'!E9)/ER!$G$7)*1000</f>
+        <v>50103111.954071276</v>
+      </c>
+      <c r="D7">
         <v>10.344016534467411</v>
       </c>
-      <c r="C7" s="49">
-        <f>(('P. Totals'!D9+'P. Totals'!E9)/ER!$G$7/Education!I15)*1000</f>
+      <c r="E7">
         <v>95.509815271607081</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:5">
       <c r="A8" s="43" t="s">
         <v>746</v>
       </c>
       <c r="B8" s="49">
-        <f>(('P. Totals'!J10+'P. Totals'!K10)/ER!$G$7/'Population data'!C25)*1000</f>
+        <f>(('P. Totals'!J10+'P. Totals'!K10)/ER!$G$7)*1000</f>
+        <v>22690940.724407803</v>
+      </c>
+      <c r="C8" s="49">
+        <f>(('P. Totals'!D10+'P. Totals'!E10)/ER!$G$7)*1000</f>
+        <v>61486827.476506099</v>
+      </c>
+      <c r="D8">
         <v>13.811348528478442</v>
       </c>
-      <c r="C8" s="49">
-        <f>(('P. Totals'!D10+'P. Totals'!E10)/ER!$G$7/Education!I16)*1000</f>
+      <c r="E8">
         <v>112.45814376236819</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:5">
       <c r="A9" s="43" t="s">
         <v>413</v>
       </c>
       <c r="B9" s="49">
-        <f>(('P. Totals'!J11+'P. Totals'!K11)/ER!$G$7/'Population data'!C26)*1000</f>
+        <f>(('P. Totals'!J11+'P. Totals'!K11))/ER!$G$7*1000</f>
+        <v>16460832.550120326</v>
+      </c>
+      <c r="C9" s="49">
+        <f>(('P. Totals'!D11+'P. Totals'!E11)/ER!$G$7)*1000</f>
+        <v>48999332.783393666</v>
+      </c>
+      <c r="D9">
         <v>12.942757965463867</v>
       </c>
-      <c r="C9" s="49">
-        <f>(('P. Totals'!D11+'P. Totals'!E11)/ER!$G$7/Education!I17)*1000</f>
+      <c r="E9">
         <v>106.72654931681808</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:5">
       <c r="A10" s="43" t="s">
         <v>444</v>
       </c>
       <c r="B10" s="49">
-        <f>(('P. Totals'!J12+'P. Totals'!K12)/ER!$G$7/'Population data'!C27)*1000</f>
+        <f>(('P. Totals'!J12+'P. Totals'!K12)/ER!$G$7)*1000</f>
+        <v>11686386.775219275</v>
+      </c>
+      <c r="C10" s="49">
+        <f>(('P. Totals'!D12+'P. Totals'!E12)/ER!$G$7)*1000</f>
+        <v>45641771.841499433</v>
+      </c>
+      <c r="D10">
         <v>9.5126199418315753</v>
       </c>
-      <c r="C10" s="49">
-        <f>(('P. Totals'!D12+'P. Totals'!E12)/ER!$G$7/Education!I18)*1000</f>
+      <c r="E10">
         <v>111.18173962339849</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:5">
       <c r="A11" s="43" t="s">
         <v>508</v>
       </c>
       <c r="B11" s="49">
-        <f>(('P. Totals'!J13+'P. Totals'!K13)/ER!$G$7/'Population data'!C28)*1000</f>
+        <f>(('P. Totals'!J13+'P. Totals'!K13)/ER!$G$7)*1000</f>
+        <v>12068091.632142643</v>
+      </c>
+      <c r="C11" s="49">
+        <f>(('P. Totals'!D13+'P. Totals'!E13)/ER!$G$7)*1000</f>
+        <v>29964086.989274845</v>
+      </c>
+      <c r="D11">
         <v>10.009124616422904</v>
       </c>
-      <c r="C11" s="49">
-        <f>(('P. Totals'!D13+'P. Totals'!E13)/ER!$G$7/Education!I19)*1000</f>
+      <c r="E11">
         <v>61.709352735919268</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:5">
       <c r="A12" s="44" t="s">
         <v>827</v>
       </c>
       <c r="B12" s="49">
-        <f>(('P. Totals'!J14+'P. Totals'!K14)/ER!$G$7/'Population data'!C29)*1000</f>
+        <f>(('P. Totals'!J14+'P. Totals'!K14)/ER!$G$7)*1000</f>
+        <v>99328938.730235308</v>
+      </c>
+      <c r="C12" s="49">
+        <f>(('P. Totals'!D14+'P. Totals'!E14)/ER!$G$7)*1000</f>
+        <v>73606574.708327532</v>
+      </c>
+      <c r="D12">
         <v>90.74218705371625</v>
       </c>
-      <c r="C12" s="49">
-        <f>(('P. Totals'!D14+'P. Totals'!E14)/ER!$G$7/Education!I20)*1000</f>
+      <c r="E12">
         <v>262.30168666417524</v>
       </c>
     </row>

</xml_diff>